<commit_message>
Se añadio la vista Aprendiz, su password es el mismo documento
</commit_message>
<xml_diff>
--- a/juicios_pendientes.xlsx
+++ b/juicios_pendientes.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,10 +427,10 @@
     <col width="22.8" customWidth="1" min="1" max="1"/>
     <col width="25.2" customWidth="1" min="2" max="2"/>
     <col width="9.6" customWidth="1" min="3" max="3"/>
-    <col width="13.2" customWidth="1" min="4" max="4"/>
-    <col width="9.6" customWidth="1" min="5" max="5"/>
-    <col width="15.6" customWidth="1" min="6" max="6"/>
-    <col width="31.2" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="16.8" customWidth="1" min="5" max="5"/>
+    <col width="176.4" customWidth="1" min="6" max="6"/>
+    <col width="324" customWidth="1" min="7" max="7"/>
     <col width="26.4" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
@@ -459,7 +459,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2556845</t>
+          <t>1262805</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>DISEÑO E INTEGRACION DE MULTIMEDIA</t>
+          <t>CONTABILIDAD Y FINANZAS</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44760</v>
+        <v>42639</v>
       </c>
     </row>
     <row r="7">
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="C7" s="1" t="n">
-        <v>45124</v>
+        <v>43368</v>
       </c>
     </row>
     <row r="8">
@@ -570,6 +570,1166 @@
       <c r="H10" t="inlineStr">
         <is>
           <t>Juicio de Evaluación</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>1 - PROMOVER LA INTERACCIÓN IDÓNEA CONSIGO MISMO, CON LOS DEMÁS Y CON LA NATURALEZA EN LOS CONTEXTOS LABORAL Y SOCIAL</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>48805 - REDIMENSIONAR PERMANENTEMENTE SU PROYECTO DE VIDA DE ACUERDO CON LAS CIRCUNSTANCIAS DEL CONTEXTO Y CON VISIÓN PROSPECTIVA.</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>1 - PROMOVER LA INTERACCIÓN IDÓNEA CONSIGO MISMO, CON LOS DEMÁS Y CON LA NATURALEZA EN LOS CONTEXTOS LABORAL Y SOCIAL</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>48806 - DESARROLLAR PROCESOS COMUNICATIVOS EFICACES Y ASERTIVOS DENTRO DE CRITERIOS DE RACIONALIDAD QUE POSIBILITEN LA CONVIVENCIA, EL ESTABLECIMIENTO DE ACUERDOS, LA CONSTRUCCIÓN COLECTIVA DEL CONOCIMIENTO Y LA RESOLUCIÓN DE PROBLEMAS DE CARÁCTER PRODUCTIVO Y SOCIAL.</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2856 - PREPARAR Y PRESENTAR LA INFORMACIÓN CONTABLE Y FINANCIERA SEGÚN NORMAS LEGALES Y POLÍTICAS ORGANIZACIONALES</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>18763 - APLICAR LAS NORMAS RELATIVAS A LA PRESENTACIÓN DE ESTADOS FINANCIEROS BÁSICOS CONFORME A LOS PRINCIPIOS DE CONTABILIDAD GENERALMENTE ACEPTADOS.</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2856 - PREPARAR Y PRESENTAR LA INFORMACIÓN CONTABLE Y FINANCIERA SEGÚN NORMAS LEGALES Y POLÍTICAS ORGANIZACIONALES</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>18764 - PREPARAR NOTAS A LOS ESTADOS FINANCIEROS PARA PRESENTACIÓN A LOS USUARIOS DE LA INFORMACIÓN.</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2856 - PREPARAR Y PRESENTAR LA INFORMACIÓN CONTABLE Y FINANCIERA SEGÚN NORMAS LEGALES Y POLÍTICAS ORGANIZACIONALES</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>18765 - ELABORAR LOS ESTADOS FINANCIEROS BÁSICOS UTILIZANDO HERRAMIENTAS INFORMÁTICAS.</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2856 - PREPARAR Y PRESENTAR LA INFORMACIÓN CONTABLE Y FINANCIERA SEGÚN NORMAS LEGALES Y POLÍTICAS ORGANIZACIONALES</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>18766 - PRESENTAR COMENTARIOS INTERPRETATIVOS A LOS ESTADOS FINANCIEROS PARA COMPLEMENTAR LA INFORMACIÓN.</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2856 - PREPARAR Y PRESENTAR LA INFORMACIÓN CONTABLE Y FINANCIERA SEGÚN NORMAS LEGALES Y POLÍTICAS ORGANIZACIONALES</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>18768 - IDENTIFICAR Y SELECCIONAR LAS CUENTAS QUE CONFORMAN LOS ESTADOS FINANCIEROS BÁSICOS DE ACUERDO AL PLAN ÚNICO DE CUENTAS.</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2863 - ESTABLECER LAS DESVIACIONES DE LA PROGRAMACIÓN FRENTE A LA EJECUCIÓN DEL PLAN FINANCIERO.</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>18779 - ANALIZAR COMPARATIVAMENTE LAS DIFERENCIAS ENTRE LA PRESUPUESTADO Y LO EJECUTADO PARA RECOMENDAR LOS AJUSTES.</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2863 - ESTABLECER LAS DESVIACIONES DE LA PROGRAMACIÓN FRENTE A LA EJECUCIÓN DEL PLAN FINANCIERO.</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>18780 - IDENTIFICAR Y DETERMINAR LAS VARIACIONES ENTRE LO EJECUTADO Y LO PRESUPUESTADO.</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2863 - ESTABLECER LAS DESVIACIONES DE LA PROGRAMACIÓN FRENTE A LA EJECUCIÓN DEL PLAN FINANCIERO.</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>18781 - ANALIZAR LOS RESULTADOS PRESUPUÉSTALES RESPECTO AL PLAN ESTRATÉGICO.</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2863 - ESTABLECER LAS DESVIACIONES DE LA PROGRAMACIÓN FRENTE A LA EJECUCIÓN DEL PLAN FINANCIERO.</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>18783 - REPROGRAMAR LAS DIFERENCIAS ENTRE LO PRESUPUESTADO Y LO EJECUTADO PARA AJUSTAR EL PLAN ESTRATÉGICO.</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2863 - ESTABLECER LAS DESVIACIONES DE LA PROGRAMACIÓN FRENTE A LA EJECUCIÓN DEL PLAN FINANCIERO.</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>18784 - CONSOLIDAR LAS VARIACIONES QUE SE PRESENTAN ENTRE EL EJECUTADO Y LO PRESUPUESTADO ANALIZAR LOS RESULTADOS PRESUPUÉSTALES.</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2863 - ESTABLECER LAS DESVIACIONES DE LA PROGRAMACIÓN FRENTE A LA EJECUCIÓN DEL PLAN FINANCIERO.</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>18785 - VALIDAR LOS RESULTADOS FINANCIEROS CON RESPECTO AL PLAN ESTRATÉGICO Y A LAS POLÍTICAS ORGANIZACIONALES.</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2864 - ANALIZAR LOS RESULTADOS CONTABLES Y FINANCIEROS SEGÚN LOS CRITERIOS DE EVALUACIÓN ESTABLECIDOS POR LA ORGANIZACIÓN</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>18769 - CONCEPTUALIZAR LA SITUACIÓN FINANCIERA DE LA EMPRESA RESPECTO AL ENTORNO ECONÓMICO Y LEGAL.</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2864 - ANALIZAR LOS RESULTADOS CONTABLES Y FINANCIEROS SEGÚN LOS CRITERIOS DE EVALUACIÓN ESTABLECIDOS POR LA ORGANIZACIÓN</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>18770 - APLICAR LOS INDICADORES FINANCIEROS PARA DETERMINAR LA LIQUIDEZ, RENTABILIDAD, NIVEL DE ENDEUDAMIENTO, ACTIVIDAD, EBITDA Y EL VALOR ECONÓMICO AGREGADO DE LA EMPRESA.</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2864 - ANALIZAR LOS RESULTADOS CONTABLES Y FINANCIEROS SEGÚN LOS CRITERIOS DE EVALUACIÓN ESTABLECIDOS POR LA ORGANIZACIÓN</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>18771 - UTILIZAR LOS ÍNDICES DE INFLACIÓN Y DEVALUACIÓN PARA REEXPRESAR LA INFORMACIÓN CONTABLE Y FINANCIERA.</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2864 - ANALIZAR LOS RESULTADOS CONTABLES Y FINANCIEROS SEGÚN LOS CRITERIOS DE EVALUACIÓN ESTABLECIDOS POR LA ORGANIZACIÓN</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>18772 - PRESENTAR RECOMENDACIONES PARA SOLUCIONAR LOS PROBLEMAS FINANCIEROS DE LA ORGANIZACIÓN.</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2864 - ANALIZAR LOS RESULTADOS CONTABLES Y FINANCIEROS SEGÚN LOS CRITERIOS DE EVALUACIÓN ESTABLECIDOS POR LA ORGANIZACIÓN</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>18773 - CONCLUIR Y PRESENTAR INFORME SOBRE LA SITUACIÓN FINANCIERA DE LA ORGANIZACIÓN PARA LA TOMA DE DECISIONES.</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2864 - ANALIZAR LOS RESULTADOS CONTABLES Y FINANCIEROS SEGÚN LOS CRITERIOS DE EVALUACIÓN ESTABLECIDOS POR LA ORGANIZACIÓN</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>18774 - INVESTIGAR Y CONCLUIR SOBRE PROBLEMAS FINANCIEROS DE LA ORGANIZACIÓN PARA APLICACIÓN DE CORRECTIVOS.</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2865 - VALIDAR LA APLICACIÓN DE LAS FASES Y PROCEDIMIENTOS DE CONTROL INTERNO DE LA GESTIÓN FINANCIERA DE ACUERDO CON POLÍTICAS ORGANIZACIONALES.</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>18741 - ELABORAR EL INFORME DE RIESGO TENIENDO EN CUENTA LOS INDICADORES DE GESTIÓN CONTABLE Y FINANCIERA</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2865 - VALIDAR LA APLICACIÓN DE LAS FASES Y PROCEDIMIENTOS DE CONTROL INTERNO DE LA GESTIÓN FINANCIERA DE ACUERDO CON POLÍTICAS ORGANIZACIONALES.</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>18742 - IDENTIFICAR LAS POLÍTICAS Y PROCEDIMIENTOS DE CONTROL INTERNO DE LA ORGANIZACIÓN PARA EVALUACIÓN DE LA GESTIÓN.</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2865 - VALIDAR LA APLICACIÓN DE LAS FASES Y PROCEDIMIENTOS DE CONTROL INTERNO DE LA GESTIÓN FINANCIERA DE ACUERDO CON POLÍTICAS ORGANIZACIONALES.</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>18743 - REPORTAR LAS INCONSISTENCIAS ENCONTRADAS SEGÚN NORMAS VIGENTES Y ORGANIZACIONALES.</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2865 - VALIDAR LA APLICACIÓN DE LAS FASES Y PROCEDIMIENTOS DE CONTROL INTERNO DE LA GESTIÓN FINANCIERA DE ACUERDO CON POLÍTICAS ORGANIZACIONALES.</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>18744 - INTERPRETAR LAS NORMAS DE AUDITORÍA GENERALMENTE ACEPTADAS PARA APLICACIÓN A LA INFORMACIÓN.</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2865 - VALIDAR LA APLICACIÓN DE LAS FASES Y PROCEDIMIENTOS DE CONTROL INTERNO DE LA GESTIÓN FINANCIERA DE ACUERDO CON POLÍTICAS ORGANIZACIONALES.</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>18745 - IDENTIFICAR LOS DIFERENTES TIPOS DE AUDITORIA SEGÚN PROCEDIMIENTOS DE AUDITORÍA.</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2865 - VALIDAR LA APLICACIÓN DE LAS FASES Y PROCEDIMIENTOS DE CONTROL INTERNO DE LA GESTIÓN FINANCIERA DE ACUERDO CON POLÍTICAS ORGANIZACIONALES.</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>18746 - VERIFICAR LA APLICACIÓN DE NORMAS DE CONTROL INTERNO VIGENTES SEGÚN POLÍTICAS DE LA ORGANIZACIÓN.</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2865 - VALIDAR LA APLICACIÓN DE LAS FASES Y PROCEDIMIENTOS DE CONTROL INTERNO DE LA GESTIÓN FINANCIERA DE ACUERDO CON POLÍTICAS ORGANIZACIONALES.</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>18747 - ELABORAR EL MAPA DE RIESGO ORGANIZACIONAL CON LAS INCONSISTENCIAS ENCONTRADAS PARA REPROGRAMACIÓN DEL CONTROL INTERNO.</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2865 - VALIDAR LA APLICACIÓN DE LAS FASES Y PROCEDIMIENTOS DE CONTROL INTERNO DE LA GESTIÓN FINANCIERA DE ACUERDO CON POLÍTICAS ORGANIZACIONALES.</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>18748 - DEMOSTRAR SEGURIDAD Y TRANSPARENCIA EN LA APLICACIÓN DE NORMAS DE AUDITORIA Y DE CONTROL INTERNO PARA LA CONFIABILIDAD DE LA INFORMACIÓN.</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2865 - VALIDAR LA APLICACIÓN DE LAS FASES Y PROCEDIMIENTOS DE CONTROL INTERNO DE LA GESTIÓN FINANCIERA DE ACUERDO CON POLÍTICAS ORGANIZACIONALES.</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>18749 - DEMOSTRAR SEGURIDAD Y TRANSPARENCIA EN LOS INFORMES DE INCONSISTENCIAS Y RIESGOS DE LA ORGANIZACIÓN PARA EL MEJORAMIENTO CONTINUO DEL CONTROL INTERNO.</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>63469617</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>GLADIS</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>OLARTE BLANCO</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>EN FORMACION</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>3226 - COMPRENDER TEXTOS EN INGLÉS EN FORMA ESCRITA Y AUDITIVA</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>48813 - REALIZAR INTERCAMBIOS SOCIALES Y PRÁCTICOS MUY BREVES, CON UN VOCABULARIO SUFICIENTE PARA HACER UNA EXPOSICIÓN O MANTENER UNA CONVERSACIÓN SENCILLA SOBRE TEMAS TÉCNICOS</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>POR EVALUAR</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agrego ojo y y cantidad de seguimientos tabla seguimientos
</commit_message>
<xml_diff>
--- a/juicios_pendientes.xlsx
+++ b/juicios_pendientes.xlsx
@@ -448,7 +448,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45366</v>
+        <v>45369</v>
       </c>
     </row>
     <row r="3">
@@ -459,7 +459,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2556845</t>
+          <t>2824078</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Me lista todos los aprendices independientemente de si estane la bse de datos, y me actualiza sus demas datos
</commit_message>
<xml_diff>
--- a/juicios_pendientes.xlsx
+++ b/juicios_pendientes.xlsx
@@ -448,7 +448,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45370</v>
+        <v>45371</v>
       </c>
     </row>
     <row r="3">
@@ -459,7 +459,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2824078</t>
+          <t>2499992</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>DISEÑO E INTEGRACION DE MULTIMEDIA</t>
+          <t>PROGRAMA DE PRUEBA</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44760</v>
+        <v>44669</v>
       </c>
     </row>
     <row r="7">
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="C7" s="1" t="n">
-        <v>45124</v>
+        <v>45490</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Se creo el modulo para registrar una empresa, y una nueva entidad asociacion que junta idaprendiz y nit de empresa
</commit_message>
<xml_diff>
--- a/juicios_pendientes.xlsx
+++ b/juicios_pendientes.xlsx
@@ -448,7 +448,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45371</v>
+        <v>45373</v>
       </c>
     </row>
     <row r="3">
@@ -459,7 +459,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2499992</t>
+          <t>2824078</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>PROGRAMA DE PRUEBA</t>
+          <t>DISEÑO E INTEGRACION DE MULTIMEDIA</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44669</v>
+        <v>44760</v>
       </c>
     </row>
     <row r="7">
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="C7" s="1" t="n">
-        <v>45490</v>
+        <v>45124</v>
       </c>
     </row>
     <row r="8">

</xml_diff>